<commit_message>
print label with order by and customer count
</commit_message>
<xml_diff>
--- a/frontend/web/labels/1/eparcel.xlsx
+++ b/frontend/web/labels/1/eparcel.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="87">
   <si>
     <t>weight</t>
   </si>
@@ -99,25 +99,85 @@
     <t>ebay_transaction_id</t>
   </si>
   <si>
-    <t>Sally Robinson</t>
-  </si>
-  <si>
-    <t>0402 762549</t>
-  </si>
-  <si>
-    <t>20 Mountain Gum Rd</t>
-  </si>
-  <si>
-    <t>CALALA</t>
+    <t>COLIN MONTAGUE</t>
+  </si>
+  <si>
+    <t>0242 578418</t>
+  </si>
+  <si>
+    <t>1B Ribbonwood Place</t>
+  </si>
+  <si>
+    <t>ALBION PARK RAIL</t>
   </si>
   <si>
     <t>New South Wales</t>
   </si>
   <si>
-    <t>121842365891-1637713725002</t>
-  </si>
-  <si>
-    <t>salee249</t>
+    <t>121842358460-1639674302002</t>
+  </si>
+  <si>
+    <t>cfm153</t>
+  </si>
+  <si>
+    <t>Laura Gannaway</t>
+  </si>
+  <si>
+    <t>08 99216832</t>
+  </si>
+  <si>
+    <t>1 Dayana Drive</t>
+  </si>
+  <si>
+    <t>Geraldton</t>
+  </si>
+  <si>
+    <t>Western Australia</t>
+  </si>
+  <si>
+    <t>121842365891-1640040448002</t>
+  </si>
+  <si>
+    <t>lauden14</t>
+  </si>
+  <si>
+    <t>Nikolas Taufatofua</t>
+  </si>
+  <si>
+    <t>04 24543354</t>
+  </si>
+  <si>
+    <t>66 Harts road</t>
+  </si>
+  <si>
+    <t>Indooroopilly</t>
+  </si>
+  <si>
+    <t>Queensland</t>
+  </si>
+  <si>
+    <t>121842365891-1640084522002</t>
+  </si>
+  <si>
+    <t>raoul3t</t>
+  </si>
+  <si>
+    <t>Alison Wood</t>
+  </si>
+  <si>
+    <t>0249 346748</t>
+  </si>
+  <si>
+    <t>91 Ferraby Dr</t>
+  </si>
+  <si>
+    <t>Metford</t>
+  </si>
+  <si>
+    <t>121921850608-1640163399002</t>
+  </si>
+  <si>
+    <t>madgecod</t>
   </si>
   <si>
     <t>field name</t>
@@ -561,7 +621,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AMK2"/>
+  <dimension ref="A1:AMK5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A2" sqref="A2"/>
@@ -1681,7 +1741,7 @@
     </row>
     <row r="2" spans="1:1025">
       <c r="A2">
-        <v>0.4</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>27</v>
@@ -1700,13 +1760,103 @@
         <v>31</v>
       </c>
       <c r="K2">
-        <v>2340</v>
+        <v>2527</v>
       </c>
       <c r="L2" t="s">
         <v>32</v>
       </c>
       <c r="N2" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1025">
+      <c r="A3">
+        <v>0.2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3"/>
+      <c r="I3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3">
+        <v>6530</v>
+      </c>
+      <c r="L3" t="s">
+        <v>39</v>
+      </c>
+      <c r="N3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1025">
+      <c r="A4">
+        <v>0.2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4"/>
+      <c r="I4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J4" t="s">
+        <v>45</v>
+      </c>
+      <c r="K4">
+        <v>4068</v>
+      </c>
+      <c r="L4" t="s">
+        <v>46</v>
+      </c>
+      <c r="N4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1025">
+      <c r="A5">
+        <v>0.4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5"/>
+      <c r="I5" t="s">
+        <v>51</v>
+      </c>
+      <c r="J5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K5">
+        <v>2323</v>
+      </c>
+      <c r="L5" t="s">
+        <v>52</v>
+      </c>
+      <c r="N5" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -2767,13 +2917,13 @@
   <sheetData>
     <row r="1" spans="1:1025">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="C1" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="D1" t="s">
         <v>11</v>
@@ -2784,10 +2934,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:1025">
@@ -2795,13 +2945,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="C3">
         <v>35</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:1025">
@@ -2809,13 +2959,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="C4">
         <v>50</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:1025">
@@ -2823,13 +2973,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="C5">
         <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:1025">
@@ -2837,13 +2987,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="C6">
         <v>50</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:1025">
@@ -2851,13 +3001,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="C7">
         <v>40</v>
       </c>
       <c r="D7" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:1025">
@@ -2865,13 +3015,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="C8">
         <v>60</v>
       </c>
       <c r="D8" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:1025">
@@ -2879,13 +3029,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="C9">
         <v>40</v>
       </c>
       <c r="D9" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:1025">
@@ -2893,13 +3043,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="C10">
         <v>50</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:1025">
@@ -2907,10 +3057,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:1025">
@@ -2918,13 +3068,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="C12">
         <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:1025">
@@ -2932,13 +3082,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="C13">
         <v>50</v>
       </c>
       <c r="D13" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:1025">
@@ -2946,10 +3096,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="D14" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:1025">
@@ -2957,10 +3107,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="D15" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:1025">
@@ -2968,10 +3118,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="D16" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:1025">
@@ -2979,13 +3129,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="C17">
         <v>35</v>
       </c>
       <c r="D17" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:1025">
@@ -2993,13 +3143,13 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="C18">
         <v>50</v>
       </c>
       <c r="D18" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:1025">
@@ -3007,13 +3157,13 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="C19">
         <v>20</v>
       </c>
       <c r="D19" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:1025">
@@ -3021,13 +3171,13 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="C20">
         <v>50</v>
       </c>
       <c r="D20" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:1025">
@@ -3035,13 +3185,13 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="C21">
         <v>40</v>
       </c>
       <c r="D21" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:1025">
@@ -3049,13 +3199,13 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="C22">
         <v>60</v>
       </c>
       <c r="D22" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:1025">
@@ -3063,13 +3213,13 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="C23">
         <v>40</v>
       </c>
       <c r="D23" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:1025">
@@ -3077,13 +3227,13 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="C24">
         <v>50</v>
       </c>
       <c r="D24" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:1025">
@@ -3091,10 +3241,10 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="D25" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:1025">
@@ -3102,13 +3252,13 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="C26">
         <v>16</v>
       </c>
       <c r="D26" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:1025">
@@ -3116,13 +3266,13 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="C27">
         <v>20</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
     </row>
     <row r="28" spans="1:1025">
@@ -3130,13 +3280,13 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="C28">
         <v>20</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>